<commit_message>
CIMP-L: Monitoring made simple
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://revwtrcom-my.sharepoint.com/personal/connor_rudmann_craftwaterinc_com/Documents/Documents/CIMP-L/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{A4FFAA7B-F2A6-4E3C-9D83-04DB42F7EE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EF824F5-9931-45E8-B1D8-7796E3F0BBD4}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{A4FFAA7B-F2A6-4E3C-9D83-04DB42F7EE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E844C4FF-0502-4D49-933E-B521D0B5A934}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{BBAA5B86-F48C-45D3-8BBF-F8F181EC99B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{BBAA5B86-F48C-45D3-8BBF-F8F181EC99B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Permittees" sheetId="1" r:id="rId1"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6F211C-A8FB-4BCD-B233-96FA5E0D6CDF}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426D08F2-1602-4396-B4A2-57B7287C7685}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>